<commit_message>
Change the Kilinochchi center capacity
</commit_message>
<xml_diff>
--- a/CenterCapacity.xlsx
+++ b/CenterCapacity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tomato-dist-OR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8556"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10824" windowHeight="5820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +410,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>157</v>
+        <v>156.12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>